<commit_message>
Change logo of export file and add PR No. and mreqf number in mif and mreqf
</commit_message>
<xml_diff>
--- a/Assembly Issuance.xlsx
+++ b/Assembly Issuance.xlsx
@@ -15,15 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>PROGEN DIESEL TECH</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+  <si>
+    <t>PROGEN Dieseltech Services Corp.</t>
   </si>
   <si>
     <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
   </si>
   <si>
     <t>ASSEMBLY ISSUANCE</t>
+  </si>
+  <si>
+    <t>Negros Occidental, Philippines 6101</t>
   </si>
   <si>
     <t>Tel. No. 476 - 7382</t>
@@ -257,11 +260,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1152525" cy="333375"/>
+    <xdr:ext cx="714375" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Sample image" descr="Sample image"/>
@@ -656,112 +659,146 @@
       <c r="AD2" s="8"/>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3"/>
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="9"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" s="5"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3" s="8"/>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="9"/>
     </row>
     <row r="5" spans="1:30">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="G5" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:30">

</xml_diff>